<commit_message>
Admin Module Pom Classes
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B66EEE0E-7793-4D98-9BEE-A78371A6E345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\GUIFramework\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2238F3B0-F6F7-45BD-8E82-A602D775D45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11620" windowHeight="6330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
     <sheet name="org" sheetId="1" r:id="rId2"/>
-    <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="product" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="152">
   <si>
     <t>TC_ID</t>
   </si>
@@ -444,13 +449,49 @@
   </si>
   <si>
     <t>faceBook_kdd</t>
+  </si>
+  <si>
+    <t>PatientName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Password Again</t>
+  </si>
+  <si>
+    <t>Ronit</t>
+  </si>
+  <si>
+    <t>WestBengal</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>neel062@co.in</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>Create_a_Patient_Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,8 +499,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +518,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,18 +563,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -801,7 +861,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1052,6 +1112,99 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D4DBFF-79C5-4313-A7CE-A0F24C5383DC}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="H2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{E1E5C2DE-B298-49A3-BF5C-4A718F3E8097}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6E95A9-5958-495C-AC30-1DA708189BFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1102,7 +1255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
   <dimension ref="A1:B100"/>
   <sheetViews>

</xml_diff>